<commit_message>
Added connector for UART adapter
</commit_message>
<xml_diff>
--- a/oresat-c3-surrogate/oresat-c3-surrogate-bom.xlsx
+++ b/oresat-c3-surrogate/oresat-c3-surrogate-bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monke\Documents\Oresat_Git\oresat-flatsat\oresat-c3-surrogate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C047ABA3-8986-4A54-9E6B-0C3EB853859B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CC9350-3EBA-40F5-98DB-FE890D3A95A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="122">
   <si>
     <t/>
   </si>
@@ -380,6 +380,18 @@
   </si>
   <si>
     <t>Littlefuse</t>
+  </si>
+  <si>
+    <t>Sullins</t>
+  </si>
+  <si>
+    <t>S5482-ND</t>
+  </si>
+  <si>
+    <t>CONN HDR 7POS 0.1 GOLD PCB R/A</t>
+  </si>
+  <si>
+    <t>PPPC071LGBN-RC</t>
   </si>
 </sst>
 </file>
@@ -711,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1080A456-B18B-4FAE-89F7-A169628CC11E}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1364,6 +1376,29 @@
       </c>
       <c r="G27" t="s">
         <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" t="s">
+        <v>121</v>
+      </c>
+      <c r="E28" t="s">
+        <v>120</v>
+      </c>
+      <c r="F28" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" t="s">
+        <v>119</v>
+      </c>
+      <c r="H28" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>